<commit_message>
fix SH688098 and SH600636 conflict
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300319.xlsx
+++ b/src/main/resources/SZ300319.xlsx
@@ -1251,6 +1251,46 @@
         <v>1022.0</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>20201123</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>915.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>20201207</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>1087.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>20201228</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>799.0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>20210105</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>927.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>